<commit_message>
Update finance tracker: Oct 1-12 dates, remove credit card payments/transfers
</commit_message>
<xml_diff>
--- a/finance-tracker/Finance_Tracker.xlsx
+++ b/finance-tracker/Finance_Tracker.xlsx
@@ -210,12 +210,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'By Category'!$A$4:$A$16</f>
+              <f>'By Category'!$A$4:$A$15</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'By Category'!$B$4:$B$16</f>
+              <f>'By Category'!$B$4:$B$15</f>
             </numRef>
           </val>
         </ser>
@@ -547,7 +547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -605,7 +605,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2025-10-12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -636,7 +636,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2025-10-12</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -667,26 +667,26 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2025-10-12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BMW</t>
+          <t>Target</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Car Payment</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Checking</t>
+          <t>Target Card</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-751</v>
+        <v>-130.36</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -698,26 +698,26 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Target</t>
+          <t>Sagtown Coffee</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Delivery &amp; Takeout</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Target Card</t>
+          <t>Amex Gold</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>-130.36</v>
+        <v>-26.14</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -729,26 +729,26 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>OpenAI</t>
+          <t>E Hampton</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Restaurants &amp; Bars</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Freedom Card</t>
+          <t>Amex Platinum</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>-217.75</v>
+        <v>-169.65</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -760,17 +760,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sagtown Coffee</t>
+          <t>Stop &amp; Shop</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Delivery &amp; Takeout</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>-26.14</v>
+        <v>-20.04</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -791,43 +791,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>E Hampton</t>
+          <t>Addepar</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Restaurants &amp; Bars</t>
+          <t>Paychecks</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Amex Platinum</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>-169.65</v>
+          <t>Checking</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>5005.08</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Shared</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
+          <t>Gray</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Salary</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2025-10-09</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Stop &amp; Shop</t>
+          <t>Bridgehampton Wine</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -837,11 +841,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Amex Gold</t>
+          <t>USAA Visa</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>-20.04</v>
+        <v>-45.68</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -853,61 +857,57 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2025-10-09</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Addepar</t>
+          <t>Citarella</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Paychecks</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Checking</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="n">
-        <v>5005.08</v>
+          <t>Amex Gold</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>-14.15</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Gray</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Salary</t>
-        </is>
-      </c>
+          <t>Shared</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2025-10-09</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bridgehampton Wine</t>
+          <t>U-Haul</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Storage Units</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>USAA Visa</t>
+          <t>Venture Card</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>-45.68</v>
+        <v>-43</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -919,26 +919,26 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Citarella</t>
+          <t>Amazon</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Amex Gold</t>
+          <t>Amazon Prime Card</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-14.15</v>
+        <v>-57.11</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -950,26 +950,26 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>U-Haul</t>
+          <t>Stop &amp; Shop</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Storage Units</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Venture Card</t>
+          <t>Amex Gold</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>-43</v>
+        <v>-69.31</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -981,26 +981,26 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Gas &amp; Car Wash</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Amazon Prime Card</t>
+          <t>Venture Card</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>-57.11</v>
+        <v>-25.63</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1012,26 +1012,26 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Stop &amp; Shop</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Amex Gold</t>
+          <t>Venture Card</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-69.31</v>
+        <v>-146.81</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1043,17 +1043,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Gas &amp; Car Wash</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>-25.63</v>
+        <v>-2.99</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1074,12 +1074,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Amazon</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1089,11 +1089,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Venture Card</t>
+          <t>Amazon Prime Card</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>-146.81</v>
+        <v>-26.97</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1105,26 +1105,26 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Villa Italian</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Delivery &amp; Takeout</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Venture Card</t>
+          <t>Sapphire Reserve</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>-2.99</v>
+        <v>-31.6</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1136,26 +1136,26 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>Citarella</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Amazon Prime Card</t>
+          <t>Amex Gold</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>-26.97</v>
+        <v>-28.91</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1167,26 +1167,26 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Villa Italian</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Delivery &amp; Takeout</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Sapphire Reserve</t>
+          <t>Freedom Card</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>-31.6</v>
+        <v>-27.21</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1198,26 +1198,26 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Citarella</t>
+          <t>Hulu</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Amex Gold</t>
+          <t>Marriott Card</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>-28.91</v>
+        <v>-12.99</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1229,26 +1229,26 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>UBER EATS</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Delivery &amp; Takeout</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Freedom Card</t>
+          <t>Amex Platinum</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>-27.21</v>
+        <v>-33.03</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1260,26 +1260,26 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Hulu</t>
+          <t>PSEG</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Electric &amp; Gas</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Marriott Card</t>
+          <t>Venture Card</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>-12.99</v>
+        <v>-264.97</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1291,57 +1291,61 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UBER EATS</t>
+          <t>Amazon</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Delivery &amp; Takeout</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Amex Platinum</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>-33.03</v>
+          <t>Amazon Prime Card</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>20.34</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>Shared</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Refund</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PSEG</t>
+          <t>Nuuly</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Electric &amp; Gas</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Venture Card</t>
+          <t>Sapphire Reserve</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>-264.97</v>
+        <v>-363.57</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1353,61 +1357,57 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>Youtube TV</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Amazon Prime Card</t>
-        </is>
-      </c>
-      <c r="E26" s="3" t="n">
-        <v>20.34</v>
+          <t>Amex Platinum</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>-82.98999999999999</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>Shared</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Refund</t>
-        </is>
-      </c>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Nuuly</t>
+          <t>Breeze Airways</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Airline</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Sapphire Reserve</t>
+          <t>Amex Platinum</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>-363.57</v>
+        <v>-175</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1419,12 +1419,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Youtube TV</t>
+          <t>OpenAI</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1434,11 +1434,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Amex Platinum</t>
+          <t>Venture Card</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>-82.98999999999999</v>
+        <v>-21.78</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1450,26 +1450,26 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Breeze Airways</t>
+          <t>Amazon</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Airline</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Amex Platinum</t>
+          <t>Amazon Prime Card</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>-175</v>
+        <v>-14.07</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1481,26 +1481,26 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OpenAI</t>
+          <t>Etsy</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Venture Card</t>
+          <t>Slate Card</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>-21.78</v>
+        <v>-10.86</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1512,26 +1512,26 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>Breeze Airways</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Airline</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Amazon Prime Card</t>
+          <t>Amex Platinum</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>-14.07</v>
+        <v>-1504.34</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1543,26 +1543,26 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Etsy</t>
+          <t>American Airlines</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Airline</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Slate Card</t>
+          <t>Amex Platinum</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>-10.86</v>
+        <v>-315.48</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1574,95 +1574,33 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Breeze Airways</t>
+          <t>Harbor Rent</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Airline</t>
+          <t>Rent</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Amex Platinum</t>
+          <t>Checking</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>-1504.34</v>
+        <v>-7500</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>Shared</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2026-01-01</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>American Airlines</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Airline</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Amex Platinum</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>-315.48</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Shared</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2026-10-01</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Harbor Rent</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Checking</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>-7500</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Shared</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>Monthly rent</t>
         </is>
@@ -1768,7 +1706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1815,7 +1753,7 @@
         <v>7500</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>0.6098607159439546</v>
+        <v>0.6620096494526505</v>
       </c>
     </row>
     <row r="5">
@@ -1828,150 +1766,137 @@
         <v>1994.82</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>0.1622083137839093</v>
+        <v>0.1760786785228181</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Car Payment</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="B6" s="8" t="n">
-        <v>751</v>
+        <v>749.75</v>
       </c>
       <c r="C6" s="9" t="n">
-        <v>0.06106738635652133</v>
+        <v>0.06617889795694996</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Electric &amp; Gas</t>
         </is>
       </c>
       <c r="B7" s="8" t="n">
-        <v>749.75</v>
+        <v>264.97</v>
       </c>
       <c r="C7" s="9" t="n">
-        <v>0.060965742903864</v>
+        <v>0.02338835957539584</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>365.71</v>
+        <v>178.09</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>0.02973762165704849</v>
+        <v>0.01571963979613634</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Electric &amp; Gas</t>
+          <t>Restaurants &amp; Bars</t>
         </is>
       </c>
       <c r="B9" s="8" t="n">
-        <v>264.97</v>
+        <v>169.65</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>0.02154597252048929</v>
+        <v>0.01497465827061895</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Car Insurance</t>
         </is>
       </c>
       <c r="B10" s="8" t="n">
-        <v>178.09</v>
+        <v>152.51</v>
       </c>
       <c r="C10" s="9" t="n">
-        <v>0.01448134598699452</v>
+        <v>0.0134617455517365</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Restaurants &amp; Bars</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="B11" s="8" t="n">
-        <v>169.65</v>
+        <v>147.96</v>
       </c>
       <c r="C11" s="9" t="n">
-        <v>0.01379504939465225</v>
+        <v>0.01306012636440189</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Car Insurance</t>
+          <t>Delivery &amp; Takeout</t>
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>152.51</v>
+        <v>90.77000000000001</v>
       </c>
       <c r="C12" s="9" t="n">
-        <v>0.012401314371815</v>
+        <v>0.008012082117442278</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Delivery &amp; Takeout</t>
+          <t>Storage Units</t>
         </is>
       </c>
       <c r="B13" s="8" t="n">
-        <v>90.77000000000001</v>
+        <v>43</v>
       </c>
       <c r="C13" s="9" t="n">
-        <v>0.007380940958164369</v>
+        <v>0.003795521990195196</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Storage Units</t>
+          <t>Gas &amp; Car Wash</t>
         </is>
       </c>
       <c r="B14" s="8" t="n">
-        <v>43</v>
+        <v>25.63</v>
       </c>
       <c r="C14" s="9" t="n">
-        <v>0.003496534771412007</v>
+        <v>0.002262307642062858</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Gas &amp; Car Wash</t>
+          <t>Music</t>
         </is>
       </c>
       <c r="B15" s="8" t="n">
-        <v>25.63</v>
+        <v>11.99</v>
       </c>
       <c r="C15" s="9" t="n">
-        <v>0.002084097353285808</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Music</t>
-        </is>
-      </c>
-      <c r="B16" s="8" t="n">
-        <v>11.99</v>
-      </c>
-      <c r="C16" s="9" t="n">
-        <v>0.0009749639978890688</v>
+        <v>0.001058332759591637</v>
       </c>
     </row>
   </sheetData>
@@ -2060,153 +1985,153 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Checking</t>
+          <t>Target Card</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>5005.08</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>8251</v>
+        <v>130.36</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>-3245.92</v>
+        <v>-130.36</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Target Card</t>
+          <t>Amex Gold</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>130.36</v>
+        <v>158.55</v>
       </c>
       <c r="D6" s="8" t="n">
-        <v>-130.36</v>
+        <v>-158.55</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Freedom Card</t>
+          <t>Amex Platinum</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>244.96</v>
+        <v>2280.49</v>
       </c>
       <c r="D7" s="8" t="n">
-        <v>-244.96</v>
+        <v>-2280.49</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Amex Gold</t>
+          <t>Checking</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>0</v>
+        <v>5005.08</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>158.55</v>
+        <v>7500</v>
       </c>
       <c r="D8" s="8" t="n">
-        <v>-158.55</v>
+        <v>-2494.92</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Amex Platinum</t>
+          <t>USAA Visa</t>
         </is>
       </c>
       <c r="B9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2280.49</v>
+        <v>45.68</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>-2280.49</v>
+        <v>-45.68</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>USAA Visa</t>
+          <t>Amazon Prime Card</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>0</v>
+        <v>20.34</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45.68</v>
+        <v>98.15000000000001</v>
       </c>
       <c r="D10" s="8" t="n">
-        <v>-45.68</v>
+        <v>-77.81</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Amazon Prime Card</t>
+          <t>Sapphire Reserve</t>
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>20.34</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>98.15000000000001</v>
+        <v>395.17</v>
       </c>
       <c r="D11" s="8" t="n">
-        <v>-77.81</v>
+        <v>-395.17</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sapphire Reserve</t>
+          <t>Freedom Card</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>395.17</v>
+        <v>27.21</v>
       </c>
       <c r="D12" s="8" t="n">
-        <v>-395.17</v>
+        <v>-27.21</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">

</xml_diff>